<commit_message>
Shifted to using TJ to report fuel outputs
</commit_message>
<xml_diff>
--- a/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
+++ b/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
@@ -1,21 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-hongkong\InputData\web-app\BpTPEU\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="14100"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BpTPEU" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>BpTPEU BTU per Total Primary Energy Unit</t>
   </si>
@@ -29,19 +44,28 @@
     <t>BTU</t>
   </si>
   <si>
-    <t>One Quadrillion BTU</t>
-  </si>
-  <si>
-    <t>For the U.S., the unit for Total Primary Energy output is quadrillion BTU.</t>
-  </si>
-  <si>
     <t>none needed</t>
   </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>For Hong Kong, the unit for Total Primary Energy output is TJ.</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>One TJ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,6 +123,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -146,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -181,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,37 +417,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>1055</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
+        <f>A11/D11*10^12</f>
+        <v>947867298.57819903</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -434,31 +504,33 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <f>10^15</f>
-        <v>1000000000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f>About!D12</f>
+        <v>947867298.57819903</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="3"/>
     </row>
   </sheetData>
@@ -467,31 +539,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
-    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
-    <xsd:import namespace="7889d872-e2a2-4afb-87bc-97561eced75f"/>
-    <xsd:import namespace="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005D5DE895D8AE54A972C2171818FD093" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85f6924c4aafd897c3f23384ae9dc35">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01f24951-2a3e-4fd5-a813-71a74687f653" xmlns:ns3="80a27e12-bb1f-4e28-b766-51f62aa5c67e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11afb4ea5aef950dd888cd3ab39ccec1" ns2:_="" ns3:_="">
+    <xsd:import namespace="01f24951-2a3e-4fd5-a813-71a74687f653"/>
+    <xsd:import namespace="80a27e12-bb1f-4e28-b766-51f62aa5c67e"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -499,24 +568,68 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="01f24951-2a3e-4fd5-a813-71a74687f653" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="18" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="19" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7889d872-e2a2-4afb-87bc-97561eced75f" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="80a27e12-bb1f-4e28-b766-51f62aa5c67e" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -535,65 +648,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c9df191c-55f2-496b-9838-9a5abe4742ad" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="14" nillable="true" ma:displayName="MediaServiceLocation" ma:description="" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="20" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="21" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -711,21 +766,42 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
+  <documentManagement/>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A18CEEEF-235B-49DB-8BBD-F9769E2B7CF5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D2D73D3-462E-4CC3-993B-219026AE3A63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="01f24951-2a3e-4fd5-a813-71a74687f653"/>
+    <ds:schemaRef ds:uri="80a27e12-bb1f-4e28-b766-51f62aa5c67e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{651AFD69-AA5F-4614-AEC0-A0DAE2B6030C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{651AFD69-AA5F-4614-AEC0-A0DAE2B6030C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B67C0D24-F5B6-480D-A2EF-F01CFA1BA16A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B67C0D24-F5B6-480D-A2EF-F01CFA1BA16A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>